<commit_message>
Finalized 21, A22 implementation needed next
</commit_message>
<xml_diff>
--- a/CompilerAssignment-A21-Specification/Apouc_TransitionTable.xlsx
+++ b/CompilerAssignment-A21-Specification/Apouc_TransitionTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b2af7fe9a94976d/Documents/GitHub/AC22CMP/CompilerAssignment-A21-Specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="14_{8FCA2C69-600D-4FA2-8E5A-024179B8B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27BB66DD-876A-4FCB-9EC8-225D9F2AFC05}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="14_{8FCA2C69-600D-4FA2-8E5A-024179B8B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B993D824-3765-49B4-9FD3-24DC7DB3147D}"/>
   <bookViews>
-    <workbookView xWindow="-6390" yWindow="1240" windowWidth="14400" windowHeight="7550" xr2:uid="{CDF9313D-D7EC-4E44-86E6-1C710AE7FB6B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{CDF9313D-D7EC-4E44-86E6-1C710AE7FB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="85">
   <si>
     <t>Input</t>
   </si>
@@ -65,21 +65,12 @@
     <t>Q(")</t>
   </si>
   <si>
-    <t>LC(/*)</t>
-  </si>
-  <si>
-    <t>RC(*/)</t>
-  </si>
-  <si>
     <t>SC(#)</t>
   </si>
   <si>
     <t>P(.)</t>
   </si>
   <si>
-    <t>E(e^)</t>
-  </si>
-  <si>
     <t>S(+|-)</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
   </si>
   <si>
     <t>S13</t>
-  </si>
-  <si>
-    <t>NOAS [13]</t>
   </si>
   <si>
     <t>S14</t>
@@ -228,41 +216,89 @@
     <t>ASNR(MNID_T) [3]</t>
   </si>
   <si>
-    <t>ASNR(KEY_T) [4]</t>
-  </si>
-  <si>
     <t>ASNR(SL_T) [6]</t>
   </si>
   <si>
     <t>ASNR(CL_T) [9]</t>
   </si>
   <si>
-    <t>ASWR(FPL_T) [12]</t>
-  </si>
-  <si>
-    <t>ASWR(FPL_T) [15]</t>
-  </si>
-  <si>
-    <t>ASWR(FPL_T) [18]</t>
-  </si>
-  <si>
-    <t>ASWR(IL_T) [19]</t>
-  </si>
-  <si>
-    <t>ASWR(IL_T) [20]</t>
-  </si>
-  <si>
     <t>ASNR(MLC_T) [21]</t>
   </si>
   <si>
     <t>ASNR(SLC_T) [23]</t>
+  </si>
+  <si>
+    <t>LC({)</t>
+  </si>
+  <si>
+    <t>RC(})</t>
+  </si>
+  <si>
+    <t>E(e)</t>
+  </si>
+  <si>
+    <t>ε</t>
+  </si>
+  <si>
+    <t>EOL (New-Line)</t>
+  </si>
+  <si>
+    <t>NOAS [12]</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>ASNR(FPL) [25]</t>
+  </si>
+  <si>
+    <t>NOAS [24]</t>
+  </si>
+  <si>
+    <t>NOAS [15]</t>
+  </si>
+  <si>
+    <t>ASNR(IL_T) [20]</t>
+  </si>
+  <si>
+    <t>ASNR(IL_T) [19]</t>
+  </si>
+  <si>
+    <t>ASNR(FPL_T) [18]</t>
+  </si>
+  <si>
+    <t>ASNR(FPL_T) [13]</t>
+  </si>
+  <si>
+    <t>ASWR(VID_T/ KEY) [4]</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>S27</t>
+  </si>
+  <si>
+    <t>S28</t>
+  </si>
+  <si>
+    <t>ASNR(FPL) [28]</t>
+  </si>
+  <si>
+    <t>NOAS [26]</t>
+  </si>
+  <si>
+    <t>NOAS [27]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +314,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,7 +354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,21 +491,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,14 +515,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,6 +551,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -792,49 +854,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C2098E-371B-490A-ADB7-C35397EC1A86}">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P16" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="17"/>
+    <col min="16" max="17" width="9.140625" style="21"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="T1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="10"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S1" s="15"/>
+      <c r="V1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="7"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -850,10 +917,10 @@
       <c r="E2" s="3">
         <v>3</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="18">
         <v>4</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="18">
         <v>5</v>
       </c>
       <c r="H2" s="3">
@@ -880,16 +947,22 @@
       <c r="O2" s="3">
         <v>13</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="19">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>15</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="13"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S2" s="13"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="10"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -904,49 +977,55 @@
         <v>8</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="P3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="S3" s="13"/>
+      <c r="V3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="13"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="6"/>
-      <c r="T3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="6"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -964,46 +1043,52 @@
         <v>20</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="4">
         <v>22</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="L4" s="4">
+        <v>26</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="6"/>
-      <c r="T4" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="10"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="13"/>
+      <c r="V4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="7"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1047,18 +1132,24 @@
       <c r="O5" s="4">
         <v>4</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="6"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="13"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P5" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>4</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="13"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="10"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
@@ -1067,151 +1158,169 @@
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L6" s="4">
         <v>2</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N6" s="4">
         <v>3</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="19">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="13"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" s="13"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" s="13"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="B9" s="4">
         <v>5</v>
@@ -1222,8 +1331,8 @@
       <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="4">
-        <v>6</v>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="F9" s="16">
         <v>5</v>
@@ -1255,65 +1364,77 @@
       <c r="O9" s="4">
         <v>5</v>
       </c>
-      <c r="P9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P9" s="19">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="19">
+        <v>5</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="13"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="S10" s="13"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4">
         <v>8</v>
@@ -1322,16 +1443,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4">
         <v>8</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>21</v>
+      <c r="F11" s="4">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <v>8</v>
       </c>
       <c r="H11" s="4">
         <v>8</v>
@@ -1357,116 +1478,134 @@
       <c r="O11" s="4">
         <v>8</v>
       </c>
-      <c r="P11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P11" s="19">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>8</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="13"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="13"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" s="13"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4">
         <v>19</v>
@@ -1510,320 +1649,362 @@
       <c r="O14" s="4">
         <v>19</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="19">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>19</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4">
+        <v>13</v>
+      </c>
+      <c r="F16" s="4">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
+        <v>13</v>
+      </c>
+      <c r="H16" s="4">
+        <v>13</v>
+      </c>
+      <c r="I16" s="4">
+        <v>13</v>
+      </c>
+      <c r="J16" s="4">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4">
+        <v>13</v>
+      </c>
+      <c r="L16" s="4">
+        <v>13</v>
+      </c>
+      <c r="M16" s="4">
+        <v>13</v>
+      </c>
+      <c r="N16" s="4">
+        <v>13</v>
+      </c>
+      <c r="O16" s="4">
+        <v>13</v>
+      </c>
+      <c r="P16" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>13</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="4">
-        <v>12</v>
-      </c>
-      <c r="C15" s="4">
-        <v>11</v>
-      </c>
-      <c r="D15" s="4">
-        <v>12</v>
-      </c>
-      <c r="E15" s="4">
-        <v>12</v>
-      </c>
-      <c r="F15" s="16">
-        <v>12</v>
-      </c>
-      <c r="G15" s="16">
-        <v>12</v>
-      </c>
-      <c r="H15" s="4">
-        <v>12</v>
-      </c>
-      <c r="I15" s="4">
-        <v>12</v>
-      </c>
-      <c r="J15" s="4">
-        <v>13</v>
-      </c>
-      <c r="K15" s="4">
-        <v>12</v>
-      </c>
-      <c r="L15" s="4">
-        <v>12</v>
-      </c>
-      <c r="M15" s="4">
-        <v>12</v>
-      </c>
-      <c r="N15" s="4">
-        <v>12</v>
-      </c>
-      <c r="O15" s="4">
-        <v>12</v>
-      </c>
-      <c r="P15" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="4">
-        <v>14</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="4">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4">
-        <v>14</v>
-      </c>
-      <c r="D18" s="4">
-        <v>15</v>
-      </c>
-      <c r="E18" s="4">
-        <v>15</v>
-      </c>
-      <c r="F18" s="16">
-        <v>15</v>
-      </c>
-      <c r="G18" s="16">
-        <v>15</v>
-      </c>
-      <c r="H18" s="4">
-        <v>15</v>
-      </c>
-      <c r="I18" s="4">
-        <v>15</v>
-      </c>
-      <c r="J18" s="4">
-        <v>15</v>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="K18" s="4">
         <v>15</v>
       </c>
-      <c r="L18" s="4">
-        <v>15</v>
-      </c>
-      <c r="M18" s="4">
-        <v>15</v>
-      </c>
-      <c r="N18" s="4">
-        <v>15</v>
-      </c>
-      <c r="O18" s="4">
-        <v>15</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="C19" s="4">
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q19" s="6"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="S19" s="13"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K20" s="4">
         <v>17</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S20" s="13"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4">
         <v>18</v>
@@ -1867,116 +2048,134 @@
       <c r="O21" s="4">
         <v>18</v>
       </c>
-      <c r="P21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P21" s="19">
+        <v>18</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>18</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="P22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="S22" s="13"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4">
         <v>20</v>
@@ -2020,65 +2219,77 @@
       <c r="O24" s="4">
         <v>20</v>
       </c>
-      <c r="P24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="19">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="19">
+        <v>20</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="S24" s="13"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S25" s="13"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="4">
         <v>22</v>
@@ -2122,96 +2333,399 @@
       <c r="O26" s="4">
         <v>22</v>
       </c>
-      <c r="P26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P26" s="19">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="19">
+        <v>23</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="S26" s="13"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="S27" s="13"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="4">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4">
+        <v>25</v>
+      </c>
+      <c r="E28" s="4">
+        <v>25</v>
+      </c>
+      <c r="F28" s="4">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4">
+        <v>25</v>
+      </c>
+      <c r="H28" s="4">
+        <v>25</v>
+      </c>
+      <c r="I28" s="4">
+        <v>25</v>
+      </c>
+      <c r="J28" s="4">
+        <v>25</v>
+      </c>
+      <c r="K28" s="4">
+        <v>25</v>
+      </c>
+      <c r="L28" s="4">
+        <v>25</v>
+      </c>
+      <c r="M28" s="4">
+        <v>25</v>
+      </c>
+      <c r="N28" s="4">
+        <v>25</v>
+      </c>
+      <c r="O28" s="4">
+        <v>25</v>
+      </c>
+      <c r="P28" s="4">
+        <v>25</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>25</v>
+      </c>
+      <c r="R28" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="S28" s="13"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="S29" s="13"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="4">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R30" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="S30" s="13"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="4">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4">
+        <v>27</v>
+      </c>
+      <c r="D31" s="4">
         <v>28</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="E31" s="4">
         <v>28</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F31" s="4">
         <v>28</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="G31" s="4">
         <v>28</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="H31" s="4">
         <v>28</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="I31" s="4">
         <v>28</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="J31" s="4">
         <v>28</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="K31" s="4">
         <v>28</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="L31" s="4">
         <v>28</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="M31" s="4">
         <v>28</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="N31" s="4">
         <v>28</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="O31" s="4">
         <v>28</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="P31" s="4">
         <v>28</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="Q31" s="4">
         <v>28</v>
       </c>
-      <c r="P27" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q27" s="6"/>
+      <c r="R31" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="S31" s="13"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="S32" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="T1:W2"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="T4:W5"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
+  <mergeCells count="36">
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="V1:Y2"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y5"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R22:S22"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>